<commit_message>
Atualizado Sprint Backlog 2
</commit_message>
<xml_diff>
--- a/docs/Sprint Backlog 2.xlsx
+++ b/docs/Sprint Backlog 2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="240" yWindow="300" windowWidth="20730" windowHeight="11700"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint1" sheetId="5" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="29">
   <si>
     <t>Product Backlog Item</t>
   </si>
@@ -48,6 +48,9 @@
     <t>Day 4</t>
   </si>
   <si>
+    <t>Closed</t>
+  </si>
+  <si>
     <t>Total</t>
   </si>
   <si>
@@ -58,6 +61,51 @@
   </si>
   <si>
     <t>Some sprint goal</t>
+  </si>
+  <si>
+    <t>Rodrigo</t>
+  </si>
+  <si>
+    <t>Douglas</t>
+  </si>
+  <si>
+    <t>Tarefa 3 - Aplicar os testes.</t>
+  </si>
+  <si>
+    <t>Tarefa 1 - Fazer a análise da estrutura</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>Como um corretor de seguros, eu quero gerar informativo seguros a vencer</t>
+  </si>
+  <si>
+    <t>Como um corretor de seguros, eu quero que o sistema consulte o valor do veículo na tabela FIPE para cálculo do valor do seguro.</t>
+  </si>
+  <si>
+    <t>Como um corretor de seguros, eu quero poder gerar propostas com os valores de franquia, informando os aditamentos e o perfil do cliente requisitante.</t>
+  </si>
+  <si>
+    <t>Como um corretor de seguros, eu quero que o sistema possua restrição de acesso, de maneira que cada usuário utilize seu login e senha para acessar e utilizar as funcionalidades do sistema.</t>
+  </si>
+  <si>
+    <t>Tarefa 2 - Desenvolvimento da tela e criação dos cálculos.</t>
+  </si>
+  <si>
+    <t>Tarefa 2 - Criar a estrutura e a tela de parâmetros e do relatório</t>
+  </si>
+  <si>
+    <t>Tarefa 2 - Integração do WS com as tabelas que registram o valor dos veículos</t>
+  </si>
+  <si>
+    <t>Tarefa 1 - Fazer a análise.</t>
+  </si>
+  <si>
+    <t>Tarefa 2 - Desenvolver a tela de login e o controle de usuários e sessões.</t>
+  </si>
+  <si>
+    <t>Adriano</t>
   </si>
 </sst>
 </file>
@@ -144,7 +192,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -158,16 +206,10 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="23">
@@ -272,24 +314,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sprint1!$F$18:$J$18</c:f>
+              <c:f>Sprint1!$F$14:$J$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>28.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -306,11 +348,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="55320576"/>
-        <c:axId val="76084864"/>
+        <c:axId val="61878272"/>
+        <c:axId val="74249856"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="55320576"/>
+        <c:axId val="61878272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -319,7 +361,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76084864"/>
+        <c:crossAx val="74249856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -327,7 +369,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76084864"/>
+        <c:axId val="74249856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -338,7 +380,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55320576"/>
+        <c:crossAx val="61878272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -373,13 +415,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>162560</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>35560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>690880</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>35560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -687,10 +729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -732,386 +774,428 @@
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="7"/>
+      <c r="B3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1">
+        <v>8</v>
+      </c>
+      <c r="F3" s="1">
+        <v>3</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="7"/>
+      <c r="B4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>2</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1">
+        <v>3</v>
+      </c>
+      <c r="G5" s="1">
+        <v>3</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="7"/>
+      <c r="B6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1">
+        <v>4</v>
+      </c>
+      <c r="G6" s="1">
+        <v>4</v>
+      </c>
+      <c r="H6" s="1">
+        <v>4</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="7"/>
+      <c r="B7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>2</v>
+      </c>
+      <c r="H7" s="1">
+        <v>2</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="1">
+        <v>3</v>
+      </c>
+      <c r="F8" s="1">
+        <v>4</v>
+      </c>
+      <c r="G8" s="1">
+        <v>4</v>
+      </c>
+      <c r="H8" s="1">
+        <v>4</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="7"/>
+      <c r="B9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="1">
+        <v>4</v>
+      </c>
+      <c r="F9" s="1">
+        <v>3</v>
+      </c>
+      <c r="G9" s="1">
+        <v>3</v>
+      </c>
+      <c r="H9" s="1">
+        <v>3</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="7"/>
+      <c r="B10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="1">
+        <v>2</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1">
+        <v>2</v>
+      </c>
+      <c r="H10" s="1">
+        <v>2</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="1">
+        <v>3</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2</v>
+      </c>
+      <c r="G11" s="1">
+        <v>2</v>
+      </c>
+      <c r="H11" s="1">
+        <v>2</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="7"/>
+      <c r="B12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="1">
+        <v>5</v>
+      </c>
+      <c r="F12" s="1">
+        <v>3</v>
+      </c>
+      <c r="G12" s="1">
+        <v>3</v>
+      </c>
+      <c r="H12" s="1">
+        <v>3</v>
+      </c>
+      <c r="I12" s="1">
+        <v>3</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="7"/>
+      <c r="B13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="1">
+        <v>3</v>
+      </c>
+      <c r="F13" s="1">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1">
+        <v>2</v>
+      </c>
+      <c r="H13" s="1">
+        <v>2</v>
+      </c>
+      <c r="I13" s="1">
+        <v>2</v>
+      </c>
+      <c r="J13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3"/>
+      <c r="B14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="2">
+        <f t="shared" ref="E14:J14" si="0">SUM(E2:E13)</f>
+        <v>42</v>
+      </c>
+      <c r="F14" s="2">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" si="0"/>
+        <v>28.5</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="I14" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="J14" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I33" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="8"/>
-      <c r="B2" s="7"/>
-      <c r="E2" s="1">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1">
-        <v>0</v>
-      </c>
-      <c r="H2" s="1">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1">
-        <v>0</v>
-      </c>
-      <c r="J2" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8"/>
-      <c r="B3" s="7"/>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0</v>
-      </c>
-      <c r="H3" s="1">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1">
-        <v>0</v>
-      </c>
-      <c r="J3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="8"/>
-      <c r="B4" s="7"/>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1">
-        <v>0</v>
-      </c>
-      <c r="J4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="8"/>
-      <c r="B5" s="7"/>
-      <c r="E5" s="1">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1">
-        <v>0</v>
-      </c>
-      <c r="J5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="8"/>
-      <c r="B6" s="7"/>
-      <c r="E6" s="1">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0</v>
-      </c>
-      <c r="H6" s="1">
-        <v>0</v>
-      </c>
-      <c r="I6" s="1">
-        <v>0</v>
-      </c>
-      <c r="J6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="8"/>
-      <c r="B7" s="7"/>
-      <c r="E7" s="1">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0</v>
-      </c>
-      <c r="G7" s="1">
-        <v>0</v>
-      </c>
-      <c r="H7" s="1">
-        <v>0</v>
-      </c>
-      <c r="I7" s="1">
-        <v>0</v>
-      </c>
-      <c r="J7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="8"/>
-      <c r="B8" s="7"/>
-      <c r="E8" s="1">
-        <v>0</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0</v>
-      </c>
-      <c r="H8" s="1">
-        <v>0</v>
-      </c>
-      <c r="I8" s="1">
-        <v>0</v>
-      </c>
-      <c r="J8" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="8"/>
-      <c r="B9" s="7"/>
-      <c r="E9" s="1">
-        <v>0</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0</v>
-      </c>
-      <c r="H9" s="1">
-        <v>0</v>
-      </c>
-      <c r="I9" s="1">
-        <v>0</v>
-      </c>
-      <c r="J9" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="8"/>
-      <c r="B10" s="7"/>
-      <c r="E10" s="1">
-        <v>0</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0</v>
-      </c>
-      <c r="H10" s="1">
-        <v>0</v>
-      </c>
-      <c r="I10" s="1">
-        <v>0</v>
-      </c>
-      <c r="J10" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="8"/>
-      <c r="E11" s="1">
-        <v>0</v>
-      </c>
-      <c r="F11" s="1">
-        <v>0</v>
-      </c>
-      <c r="G11" s="1">
-        <v>0</v>
-      </c>
-      <c r="H11" s="1">
-        <v>0</v>
-      </c>
-      <c r="I11" s="1">
-        <v>0</v>
-      </c>
-      <c r="J11" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="8"/>
-      <c r="E12" s="1">
-        <v>0</v>
-      </c>
-      <c r="F12" s="1">
-        <v>0</v>
-      </c>
-      <c r="G12" s="1">
-        <v>0</v>
-      </c>
-      <c r="H12" s="1">
-        <v>0</v>
-      </c>
-      <c r="I12" s="1">
-        <v>0</v>
-      </c>
-      <c r="J12" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="8"/>
-      <c r="E13" s="1">
-        <v>0</v>
-      </c>
-      <c r="F13" s="1">
-        <v>0</v>
-      </c>
-      <c r="G13" s="1">
-        <v>0</v>
-      </c>
-      <c r="H13" s="1">
-        <v>0</v>
-      </c>
-      <c r="I13" s="1">
-        <v>0</v>
-      </c>
-      <c r="J13" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="9"/>
-      <c r="E14" s="1">
-        <v>0</v>
-      </c>
-      <c r="F14" s="1">
-        <v>0</v>
-      </c>
-      <c r="G14" s="1">
-        <v>0</v>
-      </c>
-      <c r="H14" s="1">
-        <v>0</v>
-      </c>
-      <c r="I14" s="1">
-        <v>0</v>
-      </c>
-      <c r="J14" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="9"/>
-      <c r="B15" s="7"/>
-      <c r="E15" s="1">
-        <v>0</v>
-      </c>
-      <c r="F15" s="1">
-        <v>0</v>
-      </c>
-      <c r="G15" s="1">
-        <v>0</v>
-      </c>
-      <c r="H15" s="1">
-        <v>0</v>
-      </c>
-      <c r="I15" s="1">
-        <v>0</v>
-      </c>
-      <c r="J15" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="9"/>
-      <c r="B16" s="7"/>
-      <c r="E16" s="1">
-        <v>0</v>
-      </c>
-      <c r="F16" s="1">
-        <v>0</v>
-      </c>
-      <c r="G16" s="1">
-        <v>0</v>
-      </c>
-      <c r="H16" s="1">
-        <v>0</v>
-      </c>
-      <c r="I16" s="1">
-        <v>0</v>
-      </c>
-      <c r="J16" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="6"/>
-      <c r="B17" s="7"/>
-    </row>
-    <row r="18" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="3"/>
-      <c r="B18" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="2">
-        <f t="shared" ref="E18:J18" si="0">SUM(E2:E16)</f>
-        <v>0</v>
-      </c>
-      <c r="F18" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G18" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H18" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I18" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J18" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="1"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>12</v>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A14:A16"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="A2:A4"/>
@@ -1127,7 +1211,19 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?><ct:contentTypeSchema ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F770ABC8F9B27C4C8461F4575C23FAEA" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6f0f4afd6cc55b40f57cb0d59e49aa45" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes">
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?><p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"><documentManagement><_dlc_DocId xmlns="0d93dc7d-5998-434b-bf34-aa89b432ec07">WORK-769-153</_dlc_DocId><_dlc_DocIdUrl xmlns="0d93dc7d-5998-434b-bf34-aa89b432ec07"><Url>http://intranet/workingtogether/projects/110405/_layouts/DocIdRedir.aspx?ID=WORK-769-153</Url><Description>WORK-769-153</Description></_dlc_DocIdUrl><IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/><Last_x0020_Archive xmlns="$ListId:Shared Documents;" xsi:nil="true"/><Reason xmlns="$ListId:Shared Documents;" xsi:nil="true"></Reason></documentManagement></p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?><ct:contentTypeSchema ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F770ABC8F9B27C4C8461F4575C23FAEA" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6f0f4afd6cc55b40f57cb0d59e49aa45" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes">
 <xsd:schema targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f7c28edf12e174e47f2c7bd2736e8bd" ns2:_="" ns3:_="" ns4:_="" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0d93dc7d-5998-434b-bf34-aa89b432ec07" xmlns:ns3="$ListId:Shared Documents;" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v4">
 <xsd:import namespace="0d93dc7d-5998-434b-bf34-aa89b432ec07"/>
 <xsd:import namespace="$ListId:Shared Documents;"/>
@@ -1301,18 +1397,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?><p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"><documentManagement><_dlc_DocId xmlns="0d93dc7d-5998-434b-bf34-aa89b432ec07">WORK-769-153</_dlc_DocId><_dlc_DocIdUrl xmlns="0d93dc7d-5998-434b-bf34-aa89b432ec07"><Url>http://intranet/workingtogether/projects/110405/_layouts/DocIdRedir.aspx?ID=WORK-769-153</Url><Description>WORK-769-153</Description></_dlc_DocIdUrl><IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/><Last_x0020_Archive xmlns="$ListId:Shared Documents;" xsi:nil="true"/><Reason xmlns="$ListId:Shared Documents;" xsi:nil="true"></Reason></documentManagement></p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
@@ -1360,21 +1444,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0008E140-BD0E-4C41-947D-F18B1A1E4B6B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2B9EEEF-7393-4E57-9716-D967A23AC816}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="0d93dc7d-5998-434b-bf34-aa89b432ec07"/>
-    <ds:schemaRef ds:uri="$ListId:Shared Documents;"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1398,9 +1470,21 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2B9EEEF-7393-4E57-9716-D967A23AC816}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0008E140-BD0E-4C41-947D-F18B1A1E4B6B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="0d93dc7d-5998-434b-bf34-aa89b432ec07"/>
+    <ds:schemaRef ds:uri="$ListId:Shared Documents;"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>